<commit_message>
DEBUG ?뚯씪??Stop Loss ??異붽? ?꾨즺
- phase1_5_core.py: CSV 而щ읆 ?뺤쓽??Stop_Loss ??異붽?
- 紐⑤뱺 ?대깽??RESTART, BUY, ADD, SELL, STOP LOSS, ?ㅻ깄????Stop Loss 媛寃?怨꾩궛 諛?湲곕줉
- Stop Loss 媛寃? H * 0.19 (81% ?섎씫)
- DEBUG ?뚯씪 ?ъ깮??(51媛?肄붿씤)
- ANALYSIS ?뚯씪 ?ъ깮??(90媛?肄붿씤)
- B7 ???ㅻⅨ履쎌뿉 Stop_Loss ???꾩튂
</commit_message>
<xml_diff>
--- a/debug/ASTER_debug.xlsx
+++ b/debug/ASTER_debug.xlsx
@@ -423,7 +423,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AD27"/>
+  <dimension ref="A1:AE27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -568,20 +568,25 @@
       </c>
       <c r="AA1" s="1" t="inlineStr">
         <is>
+          <t>Stop_Loss</t>
+        </is>
+      </c>
+      <c r="AB1" s="1" t="inlineStr">
+        <is>
           <t>cutoff_price</t>
         </is>
       </c>
-      <c r="AB1" s="1" t="inlineStr">
+      <c r="AC1" s="1" t="inlineStr">
         <is>
           <t>next_buy_level_name</t>
         </is>
       </c>
-      <c r="AC1" s="1" t="inlineStr">
+      <c r="AD1" s="1" t="inlineStr">
         <is>
           <t>next_buy_level_price</t>
         </is>
       </c>
-      <c r="AD1" s="1" t="inlineStr">
+      <c r="AE1" s="1" t="inlineStr">
         <is>
           <t>next_buy_trigger_price</t>
         </is>
@@ -671,17 +676,20 @@
         <v>0.4599</v>
       </c>
       <c r="AA2" t="n">
-        <v/>
-      </c>
-      <c r="AB2" t="inlineStr">
+        <v>0.4161</v>
+      </c>
+      <c r="AB2" t="n">
+        <v/>
+      </c>
+      <c r="AC2" t="inlineStr">
         <is>
           <t>B7</t>
         </is>
       </c>
-      <c r="AC2" t="n">
+      <c r="AD2" t="n">
         <v>0.4599</v>
       </c>
-      <c r="AD2" t="n">
+      <c r="AE2" t="n">
         <v>1.945</v>
       </c>
     </row>
@@ -769,17 +777,20 @@
         <v>0.4599</v>
       </c>
       <c r="AA3" t="n">
-        <v/>
-      </c>
-      <c r="AB3" t="inlineStr">
+        <v>0.4161</v>
+      </c>
+      <c r="AB3" t="n">
+        <v/>
+      </c>
+      <c r="AC3" t="inlineStr">
         <is>
           <t>B7</t>
         </is>
       </c>
-      <c r="AC3" t="n">
+      <c r="AD3" t="n">
         <v>0.4599</v>
       </c>
-      <c r="AD3" t="n">
+      <c r="AE3" t="n">
         <v>1.9</v>
       </c>
     </row>
@@ -867,17 +878,20 @@
         <v>0.4599</v>
       </c>
       <c r="AA4" t="n">
-        <v/>
-      </c>
-      <c r="AB4" t="inlineStr">
+        <v>0.4161</v>
+      </c>
+      <c r="AB4" t="n">
+        <v/>
+      </c>
+      <c r="AC4" t="inlineStr">
         <is>
           <t>B7</t>
         </is>
       </c>
-      <c r="AC4" t="n">
+      <c r="AD4" t="n">
         <v>0.4599</v>
       </c>
-      <c r="AD4" t="n">
+      <c r="AE4" t="n">
         <v>1.681</v>
       </c>
     </row>
@@ -965,17 +979,20 @@
         <v>0.4599</v>
       </c>
       <c r="AA5" t="n">
-        <v/>
-      </c>
-      <c r="AB5" t="inlineStr">
+        <v>0.4161</v>
+      </c>
+      <c r="AB5" t="n">
+        <v/>
+      </c>
+      <c r="AC5" t="inlineStr">
         <is>
           <t>B7</t>
         </is>
       </c>
-      <c r="AC5" t="n">
+      <c r="AD5" t="n">
         <v>0.4599</v>
       </c>
-      <c r="AD5" t="n">
+      <c r="AE5" t="n">
         <v>1.321</v>
       </c>
     </row>
@@ -1069,17 +1086,20 @@
         <v>0.4599</v>
       </c>
       <c r="AA6" t="n">
-        <v/>
-      </c>
-      <c r="AB6" t="inlineStr">
+        <v>0.4161</v>
+      </c>
+      <c r="AB6" t="n">
+        <v/>
+      </c>
+      <c r="AC6" t="inlineStr">
         <is>
           <t>B1</t>
         </is>
       </c>
-      <c r="AC6" t="n">
-        <v>1.2264</v>
-      </c>
       <c r="AD6" t="n">
+        <v>1.2264</v>
+      </c>
+      <c r="AE6" t="n">
         <v>1.155</v>
       </c>
     </row>
@@ -1171,15 +1191,18 @@
         <v>0.4599</v>
       </c>
       <c r="AA7" t="n">
+        <v>0.4161</v>
+      </c>
+      <c r="AB7" t="n">
         <v>1.243935</v>
       </c>
-      <c r="AB7" t="n">
-        <v/>
-      </c>
       <c r="AC7" t="n">
         <v/>
       </c>
       <c r="AD7" t="n">
+        <v/>
+      </c>
+      <c r="AE7" t="n">
         <v/>
       </c>
     </row>
@@ -1267,17 +1290,20 @@
         <v>0.4599</v>
       </c>
       <c r="AA8" t="n">
+        <v>0.4161</v>
+      </c>
+      <c r="AB8" t="n">
         <v>1.243935</v>
       </c>
-      <c r="AB8" t="inlineStr">
+      <c r="AC8" t="inlineStr">
         <is>
           <t>B1</t>
         </is>
       </c>
-      <c r="AC8" t="n">
-        <v>1.2264</v>
-      </c>
       <c r="AD8" t="n">
+        <v>1.2264</v>
+      </c>
+      <c r="AE8" t="n">
         <v>1.155</v>
       </c>
     </row>
@@ -1371,17 +1397,20 @@
         <v>0.4599</v>
       </c>
       <c r="AA9" t="n">
+        <v>0.4161</v>
+      </c>
+      <c r="AB9" t="n">
         <v>1.243935</v>
       </c>
-      <c r="AB9" t="inlineStr">
+      <c r="AC9" t="inlineStr">
         <is>
           <t>B1</t>
         </is>
       </c>
-      <c r="AC9" t="n">
-        <v>1.2264</v>
-      </c>
       <c r="AD9" t="n">
+        <v>1.2264</v>
+      </c>
+      <c r="AE9" t="n">
         <v>1.16</v>
       </c>
     </row>
@@ -1473,15 +1502,18 @@
         <v>0.4599</v>
       </c>
       <c r="AA10" t="n">
+        <v>0.4161</v>
+      </c>
+      <c r="AB10" t="n">
         <v>1.243935</v>
       </c>
-      <c r="AB10" t="n">
-        <v/>
-      </c>
       <c r="AC10" t="n">
         <v/>
       </c>
       <c r="AD10" t="n">
+        <v/>
+      </c>
+      <c r="AE10" t="n">
         <v/>
       </c>
     </row>
@@ -1569,17 +1601,20 @@
         <v>0.4599</v>
       </c>
       <c r="AA11" t="n">
+        <v>0.4161</v>
+      </c>
+      <c r="AB11" t="n">
         <v>1.243935</v>
       </c>
-      <c r="AB11" t="inlineStr">
+      <c r="AC11" t="inlineStr">
         <is>
           <t>B1</t>
         </is>
       </c>
-      <c r="AC11" t="n">
-        <v>1.2264</v>
-      </c>
       <c r="AD11" t="n">
+        <v>1.2264</v>
+      </c>
+      <c r="AE11" t="n">
         <v>1.16</v>
       </c>
     </row>
@@ -1667,17 +1702,20 @@
         <v>0.4599</v>
       </c>
       <c r="AA12" t="n">
+        <v>0.4161</v>
+      </c>
+      <c r="AB12" t="n">
         <v>1.243935</v>
       </c>
-      <c r="AB12" t="inlineStr">
+      <c r="AC12" t="inlineStr">
         <is>
           <t>B7</t>
         </is>
       </c>
-      <c r="AC12" t="n">
+      <c r="AD12" t="n">
         <v>0.4599</v>
       </c>
-      <c r="AD12" t="n">
+      <c r="AE12" t="n">
         <v>1.352</v>
       </c>
     </row>
@@ -1765,17 +1803,20 @@
         <v>0.4599</v>
       </c>
       <c r="AA13" t="n">
+        <v>0.4161</v>
+      </c>
+      <c r="AB13" t="n">
         <v>1.243935</v>
       </c>
-      <c r="AB13" t="inlineStr">
+      <c r="AC13" t="inlineStr">
         <is>
           <t>B7</t>
         </is>
       </c>
-      <c r="AC13" t="n">
+      <c r="AD13" t="n">
         <v>0.4599</v>
       </c>
-      <c r="AD13" t="n">
+      <c r="AE13" t="n">
         <v>1.301</v>
       </c>
     </row>
@@ -1863,17 +1904,20 @@
         <v>0.4599</v>
       </c>
       <c r="AA14" t="n">
+        <v>0.4161</v>
+      </c>
+      <c r="AB14" t="n">
         <v>1.243935</v>
       </c>
-      <c r="AB14" t="inlineStr">
+      <c r="AC14" t="inlineStr">
         <is>
           <t>B7</t>
         </is>
       </c>
-      <c r="AC14" t="n">
+      <c r="AD14" t="n">
         <v>0.4599</v>
       </c>
-      <c r="AD14" t="n">
+      <c r="AE14" t="n">
         <v>1.262</v>
       </c>
     </row>
@@ -1967,17 +2011,20 @@
         <v>0.4599</v>
       </c>
       <c r="AA15" t="n">
+        <v>0.4161</v>
+      </c>
+      <c r="AB15" t="n">
         <v>1.243935</v>
       </c>
-      <c r="AB15" t="inlineStr">
+      <c r="AC15" t="inlineStr">
         <is>
           <t>B1</t>
         </is>
       </c>
-      <c r="AC15" t="n">
-        <v>1.2264</v>
-      </c>
       <c r="AD15" t="n">
+        <v>1.2264</v>
+      </c>
+      <c r="AE15" t="n">
         <v>1.183</v>
       </c>
     </row>
@@ -2069,15 +2116,18 @@
         <v>0.4599</v>
       </c>
       <c r="AA16" t="n">
+        <v>0.4161</v>
+      </c>
+      <c r="AB16" t="n">
         <v>1.243935</v>
       </c>
-      <c r="AB16" t="n">
-        <v/>
-      </c>
       <c r="AC16" t="n">
         <v/>
       </c>
       <c r="AD16" t="n">
+        <v/>
+      </c>
+      <c r="AE16" t="n">
         <v/>
       </c>
     </row>
@@ -2165,17 +2215,20 @@
         <v>0.4599</v>
       </c>
       <c r="AA17" t="n">
+        <v>0.4161</v>
+      </c>
+      <c r="AB17" t="n">
         <v>1.243935</v>
       </c>
-      <c r="AB17" t="inlineStr">
+      <c r="AC17" t="inlineStr">
         <is>
           <t>B1</t>
         </is>
       </c>
-      <c r="AC17" t="n">
-        <v>1.2264</v>
-      </c>
       <c r="AD17" t="n">
+        <v>1.2264</v>
+      </c>
+      <c r="AE17" t="n">
         <v>1.183</v>
       </c>
     </row>
@@ -2269,17 +2322,20 @@
         <v>0.4599</v>
       </c>
       <c r="AA18" t="n">
+        <v>0.4161</v>
+      </c>
+      <c r="AB18" t="n">
         <v>1.243935</v>
       </c>
-      <c r="AB18" t="inlineStr">
+      <c r="AC18" t="inlineStr">
         <is>
           <t>B1</t>
         </is>
       </c>
-      <c r="AC18" t="n">
-        <v>1.2264</v>
-      </c>
       <c r="AD18" t="n">
+        <v>1.2264</v>
+      </c>
+      <c r="AE18" t="n">
         <v>1.02</v>
       </c>
     </row>
@@ -2373,17 +2429,20 @@
         <v>0.4599</v>
       </c>
       <c r="AA19" t="n">
+        <v>0.4161</v>
+      </c>
+      <c r="AB19" t="n">
         <v>1.243935</v>
       </c>
-      <c r="AB19" t="inlineStr">
+      <c r="AC19" t="inlineStr">
         <is>
           <t>B2</t>
         </is>
       </c>
-      <c r="AC19" t="n">
-        <v>1.1388</v>
-      </c>
       <c r="AD19" t="n">
+        <v>1.1388</v>
+      </c>
+      <c r="AE19" t="n">
         <v>1.02</v>
       </c>
     </row>
@@ -2475,15 +2534,18 @@
         <v>0.4599</v>
       </c>
       <c r="AA20" t="n">
+        <v>0.4161</v>
+      </c>
+      <c r="AB20" t="n">
         <v>1.19646</v>
       </c>
-      <c r="AB20" t="n">
-        <v/>
-      </c>
       <c r="AC20" t="n">
         <v/>
       </c>
       <c r="AD20" t="n">
+        <v/>
+      </c>
+      <c r="AE20" t="n">
         <v/>
       </c>
     </row>
@@ -2571,17 +2633,20 @@
         <v>0.4599</v>
       </c>
       <c r="AA21" t="n">
+        <v>0.4161</v>
+      </c>
+      <c r="AB21" t="n">
         <v>1.19646</v>
       </c>
-      <c r="AB21" t="inlineStr">
+      <c r="AC21" t="inlineStr">
         <is>
           <t>B2</t>
         </is>
       </c>
-      <c r="AC21" t="n">
-        <v>1.1388</v>
-      </c>
       <c r="AD21" t="n">
+        <v>1.1388</v>
+      </c>
+      <c r="AE21" t="n">
         <v>1.02</v>
       </c>
     </row>
@@ -2675,17 +2740,20 @@
         <v>0.4599</v>
       </c>
       <c r="AA22" t="n">
+        <v>0.4161</v>
+      </c>
+      <c r="AB22" t="n">
         <v>1.19646</v>
       </c>
-      <c r="AB22" t="inlineStr">
+      <c r="AC22" t="inlineStr">
         <is>
           <t>B2</t>
         </is>
       </c>
-      <c r="AC22" t="n">
-        <v>1.1388</v>
-      </c>
       <c r="AD22" t="n">
+        <v>1.1388</v>
+      </c>
+      <c r="AE22" t="n">
         <v>1.121</v>
       </c>
     </row>
@@ -2777,15 +2845,18 @@
         <v>0.4599</v>
       </c>
       <c r="AA23" t="n">
+        <v>0.4161</v>
+      </c>
+      <c r="AB23" t="n">
         <v>1.19646</v>
       </c>
-      <c r="AB23" t="n">
-        <v/>
-      </c>
       <c r="AC23" t="n">
         <v/>
       </c>
       <c r="AD23" t="n">
+        <v/>
+      </c>
+      <c r="AE23" t="n">
         <v/>
       </c>
     </row>
@@ -2873,17 +2944,20 @@
         <v>0.4599</v>
       </c>
       <c r="AA24" t="n">
+        <v>0.4161</v>
+      </c>
+      <c r="AB24" t="n">
         <v>1.19646</v>
       </c>
-      <c r="AB24" t="inlineStr">
+      <c r="AC24" t="inlineStr">
         <is>
           <t>B2</t>
         </is>
       </c>
-      <c r="AC24" t="n">
-        <v>1.1388</v>
-      </c>
       <c r="AD24" t="n">
+        <v>1.1388</v>
+      </c>
+      <c r="AE24" t="n">
         <v>1.121</v>
       </c>
     </row>
@@ -2903,7 +2977,7 @@
         <v>1.117</v>
       </c>
       <c r="E25" t="n">
-        <v>1.182</v>
+        <v>1.18</v>
       </c>
       <c r="F25" t="inlineStr">
         <is>
@@ -2977,17 +3051,20 @@
         <v>0.4599</v>
       </c>
       <c r="AA25" t="n">
+        <v>0.4161</v>
+      </c>
+      <c r="AB25" t="n">
         <v>1.19646</v>
       </c>
-      <c r="AB25" t="inlineStr">
+      <c r="AC25" t="inlineStr">
         <is>
           <t>B2</t>
         </is>
       </c>
-      <c r="AC25" t="n">
-        <v>1.1388</v>
-      </c>
       <c r="AD25" t="n">
+        <v>1.1388</v>
+      </c>
+      <c r="AE25" t="n">
         <v>1.117</v>
       </c>
     </row>
@@ -3007,7 +3084,7 @@
         <v>1.117</v>
       </c>
       <c r="E26" t="n">
-        <v>1.182</v>
+        <v>1.18</v>
       </c>
       <c r="F26" t="inlineStr">
         <is>
@@ -3079,15 +3156,18 @@
         <v>0.4599</v>
       </c>
       <c r="AA26" t="n">
+        <v>0.4161</v>
+      </c>
+      <c r="AB26" t="n">
         <v>1.19646</v>
       </c>
-      <c r="AB26" t="n">
-        <v/>
-      </c>
       <c r="AC26" t="n">
         <v/>
       </c>
       <c r="AD26" t="n">
+        <v/>
+      </c>
+      <c r="AE26" t="n">
         <v/>
       </c>
     </row>
@@ -3107,7 +3187,7 @@
         <v>1.117</v>
       </c>
       <c r="E27" t="n">
-        <v>1.182</v>
+        <v>1.18</v>
       </c>
       <c r="F27" t="inlineStr">
         <is>
@@ -3175,17 +3255,20 @@
         <v>0.4599</v>
       </c>
       <c r="AA27" t="n">
+        <v>0.4161</v>
+      </c>
+      <c r="AB27" t="n">
         <v>1.19646</v>
       </c>
-      <c r="AB27" t="inlineStr">
+      <c r="AC27" t="inlineStr">
         <is>
           <t>B2</t>
         </is>
       </c>
-      <c r="AC27" t="n">
-        <v>1.1388</v>
-      </c>
       <c r="AD27" t="n">
+        <v>1.1388</v>
+      </c>
+      <c r="AE27" t="n">
         <v>1.117</v>
       </c>
     </row>

</xml_diff>